<commit_message>
TCs Updated. Element Repository and Constant updated.
</commit_message>
<xml_diff>
--- a/GroceryApp/src/main/resources/ExcelFiles/DataProvider.xlsx
+++ b/GroceryApp/src/main/resources/ExcelFiles/DataProvider.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgkri\git\GroceryApp\GroceryApp\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC2C716-7793-4C76-91DD-35F18C395500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D23DBB9-068A-4643-B711-7DD6BE4666FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DC581DA6-7CE6-4B35-A35F-4C62BE6E7C06}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DC581DA6-7CE6-4B35-A35F-4C62BE6E7C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ExpectedResult" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Username</t>
   </si>
@@ -40,19 +41,249 @@
   </si>
   <si>
     <t>abcd</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>TABLESEARCHERROR</t>
+  </si>
+  <si>
+    <t>Mismatch in Values and Search Criteria</t>
+  </si>
+  <si>
+    <t>STATUSACTIVE</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>ALERTERROR</t>
+  </si>
+  <si>
+    <t>Mismatch in Alert text</t>
+  </si>
+  <si>
+    <t>ALERTNEWUSERADDED</t>
+  </si>
+  <si>
+    <t>User Created Successfully</t>
+  </si>
+  <si>
+    <t>PAGELOADERROR</t>
+  </si>
+  <si>
+    <t>Target page is not loaded</t>
+  </si>
+  <si>
+    <t>LOGINTITLETEXT</t>
+  </si>
+  <si>
+    <t>7rmart supermarket</t>
+  </si>
+  <si>
+    <t>EXPENSECATTITLE</t>
+  </si>
+  <si>
+    <t>Expense Category</t>
+  </si>
+  <si>
+    <t>MANAGEDELIVERYBOYTITLE</t>
+  </si>
+  <si>
+    <t>List Delivery Boy</t>
+  </si>
+  <si>
+    <t>MOBILESLIDERTITLE</t>
+  </si>
+  <si>
+    <t>List Mobile Sliders</t>
+  </si>
+  <si>
+    <t>SIGNINTEXT</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>SIGNINBUTTONERROR</t>
+  </si>
+  <si>
+    <t>Text of Sign-In button is mismatched</t>
+  </si>
+  <si>
+    <t>CHECKBOXERROR</t>
+  </si>
+  <si>
+    <t>Error in checkbox selection status</t>
+  </si>
+  <si>
+    <t>LOGINERROR</t>
+  </si>
+  <si>
+    <t>Login Failed</t>
+  </si>
+  <si>
+    <t>INVALIDUSERNAMEALERT</t>
+  </si>
+  <si>
+    <t>Invalid Username/Password</t>
+  </si>
+  <si>
+    <t>LOGINTITLE</t>
+  </si>
+  <si>
+    <t>Mismatch in Login page title</t>
+  </si>
+  <si>
+    <t>SIGNINBGCOLOR</t>
+  </si>
+  <si>
+    <t>rgba(52, 58, 64, 1)</t>
+  </si>
+  <si>
+    <t>BACKGROUNDCOLORERROR</t>
+  </si>
+  <si>
+    <t>Mismatch in Background color</t>
+  </si>
+  <si>
+    <t>USERNAMEERROR</t>
+  </si>
+  <si>
+    <t>Username field is not selected</t>
+  </si>
+  <si>
+    <t>REMEMBERMELABEL</t>
+  </si>
+  <si>
+    <t>Remember Me</t>
+  </si>
+  <si>
+    <t>NEWCATEGORYALERT</t>
+  </si>
+  <si>
+    <t>Sub Category Created Successfully</t>
+  </si>
+  <si>
+    <t>SUBCATEGORYUPDATEERROR</t>
+  </si>
+  <si>
+    <t>Sub Category update not successful</t>
+  </si>
+  <si>
+    <t>DELETESUBCATALERT</t>
+  </si>
+  <si>
+    <t>Do you want to delete this Sub Category?</t>
+  </si>
+  <si>
+    <t>MANAGECONTENTPAGEEDITALERT</t>
+  </si>
+  <si>
+    <t>Page Updated Successfully</t>
+  </si>
+  <si>
+    <t>UPDATEDATAERROR</t>
+  </si>
+  <si>
+    <t>Updated data is not reflected correctly</t>
+  </si>
+  <si>
+    <t>DELIVERYBOYUSERNAME</t>
+  </si>
+  <si>
+    <t>Trudie01</t>
+  </si>
+  <si>
+    <t>EXPECTEDTEXTERROR</t>
+  </si>
+  <si>
+    <t>Expected text is not present in the element</t>
+  </si>
+  <si>
+    <t>ELEMENTPRESENCEERROR</t>
+  </si>
+  <si>
+    <t>Element is not present</t>
+  </si>
+  <si>
+    <t>STATUSINACTIVE</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>FOOTERPAGETITLE</t>
+  </si>
+  <si>
+    <t>Footer Text</t>
+  </si>
+  <si>
+    <t>ERRORINDELIVERYCHARGE</t>
+  </si>
+  <si>
+    <t>Delivery Charge is not same across the State</t>
+  </si>
+  <si>
+    <t>PAYMENTLIMITUPDATEALERT</t>
+  </si>
+  <si>
+    <t>Payment Method Updated Successfully</t>
+  </si>
+  <si>
+    <t>LISTPRODUCTCATEGORYERROR</t>
+  </si>
+  <si>
+    <t>Mismatch in List Products Category and Search Criteria</t>
+  </si>
+  <si>
+    <t>MOBILESLIDERALERT</t>
+  </si>
+  <si>
+    <t>Mobile Slider Created Successfully</t>
+  </si>
+  <si>
+    <t>MOBILESLIDERDELETEALERT</t>
+  </si>
+  <si>
+    <t>Do you want to delete this Mobile Slider?</t>
+  </si>
+  <si>
+    <t>PUSHNOTIFICATIONALERT</t>
+  </si>
+  <si>
+    <t>Message send successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF0000C0"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,8 +306,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5151A348-04E9-41E7-AC6D-EE74A161233B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -426,4 +663,312 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2AECBB-AA45-4CD8-A7A8-E0E0B71F62AA}">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>